<commit_message>
Updating Zeus v2 report template with detail test cases
</commit_message>
<xml_diff>
--- a/App_Release/Zeus_Testing_template.xlsx
+++ b/App_Release/Zeus_Testing_template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\001-Github\RYSE_Testing_record\App_Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CB2F7B-43D7-4274-B730-C98431BCDCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9C0D04-0976-45F0-9666-1DF6E79EAF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
+    <workbookView xWindow="768" yWindow="852" windowWidth="21600" windowHeight="11232" activeTab="2" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Bridge" sheetId="2" r:id="rId2"/>
+    <sheet name="AX_Account" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="175">
   <si>
     <t>Code</t>
   </si>
@@ -531,6 +532,69 @@
   </si>
   <si>
     <t>Valid ChangeTimezone</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>Verify the RYSE App Account Login and Logout Feature</t>
+  </si>
+  <si>
+    <t>Reset App</t>
+  </si>
+  <si>
+    <t>LogIn</t>
+  </si>
+  <si>
+    <t>LogOut</t>
+  </si>
+  <si>
+    <t>Validate the RYSE app's responses by using different combinations of account and password to log in</t>
+  </si>
+  <si>
+    <t>LogIn Negative</t>
+  </si>
+  <si>
+    <t>Verify the RYSE App Sign up feature with a unique non-existing email address &amp; a valid password</t>
+  </si>
+  <si>
+    <t>SignUp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the RYSE app's responses by using different combinations of account and password to sign up for the account </t>
+  </si>
+  <si>
+    <t>SignUp Negative</t>
+  </si>
+  <si>
+    <t>Verify the RYSE App Account Change Password feature, but not able to submit the new password because Google blocked the Gmail access to get the verification code.</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>Verify the RYSE App profile feature in the Dashboard</t>
+  </si>
+  <si>
+    <t>View Profile</t>
+  </si>
+  <si>
+    <t>Verify the RYSE App Reset Password feature, but I can't submit the new password because Google blocked Gmail access to get the verification code.</t>
+  </si>
+  <si>
+    <t>Forget Password</t>
+  </si>
+  <si>
+    <t>Verify the RYSE App Account Login and Logout Feature with a Capital email address as the account. Android = Valid, IOS = Invalid</t>
+  </si>
+  <si>
+    <t>LogIn Capitial</t>
+  </si>
+  <si>
+    <t>Pair Bridge</t>
+  </si>
+  <si>
+    <t>Delete Bridge</t>
   </si>
 </sst>
 </file>
@@ -586,7 +650,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -635,6 +699,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -676,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -700,40 +770,22 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="190">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill>
@@ -938,1206 +990,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7EFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB1E0FD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAED4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EDCF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3D2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8DBFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFCBF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFCBF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFCBF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5B9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDFF2EB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9E5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9DC6DF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8A9FC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5D9F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5EFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEACAFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC9C1FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF72DFDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF6DEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2163,6 +1015,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>363819</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>150999</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89E49E9E-3AE8-4000-899F-EBFF435AFFA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1844040"/>
+          <a:ext cx="13394019" cy="3610479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>316188</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>120466</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB664C96-25D9-4C3A-9A0C-668AA5445442}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5486400"/>
+          <a:ext cx="13346388" cy="3229426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2484,7 +1429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA5EB23-85E7-4EC6-9FFB-9E2F32772CB4}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
@@ -2498,13 +1443,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="17" t="s">
         <v>113</v>
       </c>
@@ -3063,16 +2008,16 @@
       <c r="F49" s="19"/>
     </row>
     <row r="50" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
     </row>
     <row r="51" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
@@ -3270,16 +2215,16 @@
       <c r="F69" s="7"/>
     </row>
     <row r="70" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="26" t="s">
+      <c r="A70" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B70" s="26" t="s">
+      <c r="B70" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C70" s="27"/>
-      <c r="D70" s="26"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="25"/>
     </row>
     <row r="71" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
@@ -3429,52 +2374,44 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="CB0">
+    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="CB0">
       <formula>NOT(ISERROR(SEARCH("CB0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="CR0">
+    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="CR0">
       <formula>NOT(ISERROR(SEARCH("CR0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="CG0">
+    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="CG0">
       <formula>NOT(ISERROR(SEARCH("CG0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="CX0">
+    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="CX0">
       <formula>NOT(ISERROR(SEARCH("CX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="MX0">
+    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="MX0">
       <formula>NOT(ISERROR(SEARCH("MX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="OT0">
+    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="OT0">
       <formula>NOT(ISERROR(SEARCH("OT0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="CS0">
+    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="CS0">
       <formula>NOT(ISERROR(SEARCH("CS0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="RX0">
+    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="RX0">
       <formula>NOT(ISERROR(SEARCH("RX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="GX0">
+    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="GX0">
       <formula>NOT(ISERROR(SEARCH("GX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="12" operator="containsText" text="SB0">
+    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="SB0">
       <formula>NOT(ISERROR(SEARCH("SB0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="13" operator="containsText" text="SX0">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="SX0">
       <formula>NOT(ISERROR(SEARCH("SX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="14" operator="containsText" text="BX0">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="BX0">
       <formula>NOT(ISERROR(SEARCH("BX0",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="15" operator="containsText" text="AX0">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="AX0">
       <formula>NOT(ISERROR(SEARCH("AX0",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D87:D1048576 D1:D84">
-    <cfRule type="cellIs" dxfId="1" priority="16" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
-      <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:F1048576">
@@ -3489,6 +2426,14 @@
           <x14:id>{3E9BFF79-6FA6-4436-8241-E21D739BAB05}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D84 D87:D1048576">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+      <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3588,4 +2533,329 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6038532D-9D7B-4135-B3B3-AADD6C5932D5}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="135.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:K1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:A9">
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="CB0">
+      <formula>NOT(ISERROR(SEARCH("CB0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="CR0">
+      <formula>NOT(ISERROR(SEARCH("CR0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="CG0">
+      <formula>NOT(ISERROR(SEARCH("CG0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="CX0">
+      <formula>NOT(ISERROR(SEARCH("CX0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="MX0">
+      <formula>NOT(ISERROR(SEARCH("MX0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="OT0">
+      <formula>NOT(ISERROR(SEARCH("OT0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="CS0">
+      <formula>NOT(ISERROR(SEARCH("CS0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="RX0">
+      <formula>NOT(ISERROR(SEARCH("RX0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="GX0">
+      <formula>NOT(ISERROR(SEARCH("GX0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="SB0">
+      <formula>NOT(ISERROR(SEARCH("SB0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="SX0">
+      <formula>NOT(ISERROR(SEARCH("SX0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="13" operator="containsText" text="BX0">
+      <formula>NOT(ISERROR(SEARCH("BX0",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="14" operator="containsText" text="AX0">
+      <formula>NOT(ISERROR(SEARCH("AX0",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B9">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="formula" val="MOD(ROW(),2)=0"/>
+        <cfvo type="max"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{617BC038-0D6D-4C35-A256-368EB1B6A178}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{617BC038-0D6D-4C35-A256-368EB1B6A178}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="formula">
+                <xm:f>MOD(ROW(),2)=0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor theme="0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B1:B9</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>